<commit_message>
Correcciones generales, actualización de vistas y datos
</commit_message>
<xml_diff>
--- a/datos de flota/1765418401041_Flota_Ecorent.xlsx
+++ b/datos de flota/1765418401041_Flota_Ecorent.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J18"/>
+  <dimension ref="A1:J19"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -532,7 +532,7 @@
         <v>veh_1765502675870_3_d333phqbv</v>
       </c>
       <c r="C5" t="str">
-        <v>bus</v>
+        <v/>
       </c>
       <c r="D5" t="str">
         <v>Citroen</v>
@@ -544,13 +544,16 @@
         <v/>
       </c>
       <c r="G5" t="str">
-        <v>Sin especificar</v>
+        <v/>
       </c>
       <c r="H5" t="str">
-        <v>Sin especificar</v>
+        <v/>
+      </c>
+      <c r="I5" t="str">
+        <v/>
       </c>
       <c r="J5" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
@@ -578,6 +581,9 @@
       <c r="H6" t="str">
         <v>Sin especificar</v>
       </c>
+      <c r="I6" t="str">
+        <v>Hola</v>
+      </c>
       <c r="J6" t="b">
         <v>0</v>
       </c>
@@ -695,7 +701,7 @@
         <v>Sin especificar</v>
       </c>
       <c r="J10" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11">
@@ -753,7 +759,7 @@
         <v>Sin especificar</v>
       </c>
       <c r="J12" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13">
@@ -782,7 +788,7 @@
         <v>Sin especificar</v>
       </c>
       <c r="J13" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14">
@@ -811,7 +817,7 @@
         <v>Sin especificar</v>
       </c>
       <c r="J14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15">
@@ -869,7 +875,7 @@
         <v>Sin especificar</v>
       </c>
       <c r="J16" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="17">
@@ -912,7 +918,7 @@
         <v>camioneta</v>
       </c>
       <c r="D18" t="str">
-        <v>Great_Wall</v>
+        <v>Great Wall</v>
       </c>
       <c r="E18" t="str">
         <v>Poer 2.0</v>
@@ -927,12 +933,38 @@
         <v>Sin especificar</v>
       </c>
       <c r="J18" t="b">
-        <v>0</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>veh_1766019874075_3802</v>
+      </c>
+      <c r="C19" t="str">
+        <v>camioneta</v>
+      </c>
+      <c r="D19" t="str">
+        <v>Toyota</v>
+      </c>
+      <c r="E19" t="str">
+        <v>Hilux 2.4</v>
+      </c>
+      <c r="F19" t="str">
+        <v>dasdas</v>
+      </c>
+      <c r="G19" t="str">
+        <v>dasd</v>
+      </c>
+      <c r="H19" t="str">
+        <v>sadas</v>
+      </c>
+      <c r="I19" t="str">
+        <v/>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:J18"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:J19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>